<commit_message>
Add new translated snuggets, update translation files, and use new strings
</commit_message>
<xml_diff>
--- a/translations/RUS/site-ui-strings_RUS.xlsx
+++ b/translations/RUS/site-ui-strings_RUS.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olga.Kardanova\Desktop\Projects\91709\91709 - 04 Layout\RUS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melinda/seattle-ready/translations/RUS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <r>
       <rPr>
@@ -843,13 +843,44 @@
   </si>
   <si>
     <t>Узнайте, какие бедствия обрушивались на {{ location.area_name }} в прошлом, какое влияние они оказали и где они происходили.</t>
+  </si>
+  <si>
+    <t>Update</t>
+  </si>
+  <si>
+    <t>Обновить</t>
+  </si>
+  <si>
+    <t>Results for this location…</t>
+  </si>
+  <si>
+    <t>Результаты для этого местоположения…</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Язык</t>
+  </si>
+  <si>
+    <t>Your address, your city</t>
+  </si>
+  <si>
+    <t>Ваш адрес, ваш город</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -892,20 +923,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,22 +1218,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="75.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="75.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="75.625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="75.625" style="1"/>
+    <col min="1" max="1" width="75.6640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="75.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>57</v>
       </c>
@@ -1209,7 +1241,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
@@ -1217,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
@@ -1225,7 +1257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
@@ -1233,7 +1265,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>61</v>
       </c>
@@ -1241,7 +1273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -1249,7 +1281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
@@ -1257,7 +1289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>64</v>
       </c>
@@ -1265,7 +1297,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="126" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -1273,7 +1305,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
@@ -1281,7 +1313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>67</v>
       </c>
@@ -1289,7 +1321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>68</v>
       </c>
@@ -1297,7 +1329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>69</v>
       </c>
@@ -1305,7 +1337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -1313,7 +1345,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>71</v>
       </c>
@@ -1321,7 +1353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>72</v>
       </c>
@@ -1329,7 +1361,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>73</v>
       </c>
@@ -1337,7 +1369,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>74</v>
       </c>
@@ -1345,7 +1377,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
@@ -1353,7 +1385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>76</v>
       </c>
@@ -1361,7 +1393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>77</v>
       </c>
@@ -1369,7 +1401,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
@@ -1377,7 +1409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>79</v>
       </c>
@@ -1385,7 +1417,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>80</v>
       </c>
@@ -1393,7 +1425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>81</v>
       </c>
@@ -1401,7 +1433,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>82</v>
       </c>
@@ -1409,7 +1441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>83</v>
       </c>
@@ -1417,7 +1449,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
@@ -1425,7 +1457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>85</v>
       </c>
@@ -1433,7 +1465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>86</v>
       </c>
@@ -1441,7 +1473,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>87</v>
       </c>
@@ -1449,7 +1481,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>88</v>
       </c>
@@ -1457,7 +1489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>89</v>
       </c>
@@ -1465,7 +1497,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>90</v>
       </c>
@@ -1473,7 +1505,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>91</v>
       </c>
@@ -1481,7 +1513,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>92</v>
       </c>
@@ -1489,7 +1521,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>93</v>
       </c>
@@ -1497,7 +1529,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>94</v>
       </c>
@@ -1505,7 +1537,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" ht="96" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>95</v>
       </c>
@@ -1513,7 +1545,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>96</v>
       </c>
@@ -1521,7 +1553,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>97</v>
       </c>
@@ -1529,7 +1561,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>98</v>
       </c>
@@ -1537,7 +1569,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>99</v>
       </c>
@@ -1545,7 +1577,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>100</v>
       </c>
@@ -1553,7 +1585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>101</v>
       </c>
@@ -1561,7 +1593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>102</v>
       </c>
@@ -1569,7 +1601,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>103</v>
       </c>
@@ -1577,7 +1609,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>104</v>
       </c>
@@ -1585,7 +1617,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>105</v>
       </c>
@@ -1593,7 +1625,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>106</v>
       </c>
@@ -1601,7 +1633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>107</v>
       </c>
@@ -1609,7 +1641,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
@@ -1617,7 +1649,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>109</v>
       </c>
@@ -1625,7 +1657,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>110</v>
       </c>
@@ -1633,7 +1665,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>111</v>
       </c>
@@ -1641,7 +1673,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>112</v>
       </c>
@@ -1649,7 +1681,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>113</v>
       </c>
@@ -1657,7 +1689,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>114</v>
       </c>
@@ -1665,7 +1697,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>115</v>
       </c>
@@ -1673,21 +1705,52 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>56</v>
       </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="75" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add translations to site UI
</commit_message>
<xml_diff>
--- a/translations/RUS/site-ui-strings_RUS.xlsx
+++ b/translations/RUS/site-ui-strings_RUS.xlsx
@@ -953,7 +953,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -969,6 +969,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,7 +1256,7 @@
   <dimension ref="A1:B67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:B67"/>
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="75.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1764,7 +1765,7 @@
       <c r="A63" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1796,7 +1797,7 @@
       <c r="A67" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="7" t="s">
         <v>132</v>
       </c>
     </row>

</xml_diff>